<commit_message>
fix: conserta erro e comenta o código
</commit_message>
<xml_diff>
--- a/dados_empresas_reclameaqui.xlsx
+++ b/dados_empresas_reclameaqui.xlsx
@@ -483,7 +483,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>73.5%</t>
+          <t>73.4%</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -542,12 +542,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>97.9%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>72.8%</t>
+          <t>72.7%</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -589,7 +589,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2.75</t>
+          <t>2.74</t>
         </is>
       </c>
     </row>
@@ -643,17 +643,17 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>31.5%</t>
+          <t>31.4%</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>60.9%</t>
+          <t>60.5%</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>3.28</t>
+          <t>3.26</t>
         </is>
       </c>
     </row>

</xml_diff>